<commit_message>
Improved Notes.csv + Delay Read from XLSX file
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252A3F98-54CF-4EB4-8668-352347C20F91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FB3560-1C7B-43BF-8EE0-501467D98582}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Phase 1 Folder</t>
   </si>
@@ -43,37 +43,22 @@
     <t>Normalization Script Folder</t>
   </si>
   <si>
-    <t>D:\git\POC\Phase1</t>
-  </si>
-  <si>
-    <t>D:\git\POC\Phase1\Backend\node-neurosky</t>
-  </si>
-  <si>
-    <t>D:\git\POC\Phase1\Backend\facial-emotion-analyzer</t>
-  </si>
-  <si>
-    <t>D:\git\POC\Phase1\Reports</t>
-  </si>
-  <si>
-    <t>D:\git\POC\Phase1\Backend\data-cleaner</t>
-  </si>
-  <si>
     <t>C:\Users\InterviewRoom1\Phase1</t>
   </si>
   <si>
     <t>C:\Users\InterviewRoom1\Phase1\Backend\node-neurosky</t>
   </si>
   <si>
-    <t>C:\Users\InterviewRoom1\Phase1\Backend\facial-emotion-analyzer</t>
-  </si>
-  <si>
-    <t>C:\Users\InterviewRoom1\Phase1\Videos\alexa_funny.mp4</t>
+    <t>C:\Users\InterviewRoom1\Phase1\Backend\emotions</t>
   </si>
   <si>
     <t>C:\Users\InterviewRoom1\Phase1\Reports</t>
   </si>
   <si>
-    <t>C:\Users\InterviewRoom1\Phase1\Backend\data-cleaner</t>
+    <t>C:\Users\InterviewRoom1\Phase1\Backend\data-normalizer</t>
+  </si>
+  <si>
+    <t>C:\Users\InterviewRoom1\Phase1\Videos\men.mp4</t>
   </si>
 </sst>
 </file>
@@ -392,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,47 +417,24 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="1">
-        <v>1.1574074074074073E-4</v>
+        <v>2.5462962962962961E-4</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes in creation of notes file
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FB3560-1C7B-43BF-8EE0-501467D98582}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A63F49-8C10-4077-9818-3A542F8251DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,8 +379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1">
-        <v>2.5462962962962961E-4</v>
+        <v>1.0416666666666667E-3</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Addition of Yes/No Button to UX Testing Flow
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A63F49-8C10-4077-9818-3A542F8251DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F00469-3DD5-4A4B-B3B4-B9A74F3BC866}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1">
-        <v>1.0416666666666667E-3</v>
+        <v>2.5462962962962961E-4</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Parameters will now point to C://Phase1/ Location by default
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F00469-3DD5-4A4B-B3B4-B9A74F3BC866}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E278E308-BE7C-4965-AF6C-2DC01121C963}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,22 +43,22 @@
     <t>Normalization Script Folder</t>
   </si>
   <si>
-    <t>C:\Users\InterviewRoom1\Phase1</t>
-  </si>
-  <si>
-    <t>C:\Users\InterviewRoom1\Phase1\Backend\node-neurosky</t>
-  </si>
-  <si>
-    <t>C:\Users\InterviewRoom1\Phase1\Backend\emotions</t>
-  </si>
-  <si>
-    <t>C:\Users\InterviewRoom1\Phase1\Reports</t>
-  </si>
-  <si>
-    <t>C:\Users\InterviewRoom1\Phase1\Backend\data-normalizer</t>
-  </si>
-  <si>
-    <t>C:\Users\InterviewRoom1\Phase1\Videos\men.mp4</t>
+    <t>C:\Phase1\Backend\emotions</t>
+  </si>
+  <si>
+    <t>C:\Phase1</t>
+  </si>
+  <si>
+    <t>C:\Phase1\Backend\node-neurosky</t>
+  </si>
+  <si>
+    <t>C:\Phase1\Videos\men.mp4</t>
+  </si>
+  <si>
+    <t>C:\Phase1\Reports</t>
+  </si>
+  <si>
+    <t>C:\Phase1\Backend\data-normalizer</t>
   </si>
 </sst>
 </file>
@@ -379,15 +379,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
   </cols>
@@ -417,25 +418,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>2.5462962962962961E-4</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handled multiple checks for screen recorder
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E278E308-BE7C-4965-AF6C-2DC01121C963}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63F853B-73AA-43FD-9598-0F6686F08BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,13 +52,13 @@
     <t>C:\Phase1\Backend\node-neurosky</t>
   </si>
   <si>
-    <t>C:\Phase1\Videos\men.mp4</t>
-  </si>
-  <si>
     <t>C:\Phase1\Reports</t>
   </si>
   <si>
     <t>C:\Phase1\Backend\data-normalizer</t>
+  </si>
+  <si>
+    <t>C:\Phase1\Videos\Men Will Be Men - edited.mp4</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,16 +427,16 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>8.9120370370370362E-4</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
-        <v>2.5462962962962961E-4</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renaming video and length of demo video
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63F853B-73AA-43FD-9598-0F6686F08BDA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFBCE43-62DF-4825-9A16-02789C0EFD70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <t>C:\Phase1\Backend\data-normalizer</t>
   </si>
   <si>
-    <t>C:\Phase1\Videos\Men Will Be Men - edited.mp4</t>
+    <t>C:\Phase1\Videos\demo.mp4</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1">
-        <v>8.9120370370370362E-4</v>
+        <v>1.0763888888888889E-3</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
flow change for UX Testing + Bug Fixes
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFBCE43-62DF-4825-9A16-02789C0EFD70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0C9DBF-34D9-46ED-9939-86915139C8D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Phase 1 Folder</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>C:\Phase1\Videos\demo.mp4</t>
+  </si>
+  <si>
+    <t>Path to User Video</t>
+  </si>
+  <si>
+    <t>C:\Phase1\Backend\user-video</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -393,7 +399,7 @@
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,8 +421,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -430,13 +439,16 @@
         <v>12</v>
       </c>
       <c r="E2" s="1">
-        <v>1.0763888888888889E-3</v>
+        <v>1.0416666666666667E-3</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addition of Mouse Capture Events
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A1E2AB-0EE1-4749-B205-D1B74A02253C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C107AC-3A1D-4ACB-A85F-FE1AD922E2F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,10 +61,10 @@
     <t>C:\Phase1\Videos\demo.mp4</t>
   </si>
   <si>
-    <t>Path to User Video</t>
-  </si>
-  <si>
-    <t>C:\Phase1\Backend\user-video</t>
+    <t>Path to Mouse</t>
+  </si>
+  <si>
+    <t>C:\Phase1\Backend\mouse_clicks</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>